<commit_message>
Correct titles which initially used ASCII encoding
</commit_message>
<xml_diff>
--- a/tests/bin/sample_COUNTER_R5_reports/sample_TR_reports.xlsx
+++ b/tests/bin/sample_COUNTER_R5_reports/sample_TR_reports.xlsx
@@ -1190,9 +1190,6 @@
     <t>978-0-8223-7897-6</t>
   </si>
   <si>
-    <t>Pikachu's Global Adventure&lt;subtitle&gt;The Rise and Fall of PokÃ©mon&lt;/subtitle&gt;</t>
-  </si>
-  <si>
     <t>10.1215/9780822385813</t>
   </si>
   <si>
@@ -1200,9 +1197,6 @@
   </si>
   <si>
     <t>978-0-8223-8581-3</t>
-  </si>
-  <si>
-    <t>The Gloria AnzaldÃºa Reader</t>
   </si>
   <si>
     <t>10.1215/9780822391272</t>
@@ -1224,6 +1218,12 @@
   </si>
   <si>
     <t>978-0-8223-1536-0</t>
+  </si>
+  <si>
+    <t>Pikachu's Global Adventure&lt;subtitle&gt;The Rise and Fall of Pokémon&lt;/subtitle&gt;</t>
+  </si>
+  <si>
+    <t>The Gloria Anzaldúa Reader</t>
   </si>
 </sst>
 </file>
@@ -73909,7 +73909,7 @@
   <dimension ref="A1:AC37"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H36" sqref="H36"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -74835,7 +74835,7 @@
     </row>
     <row r="25" spans="1:29">
       <c r="A25" s="15" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>280</v>
@@ -74844,13 +74844,13 @@
         <v>280</v>
       </c>
       <c r="E25" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="F25" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="G25" s="15" t="s">
         <v>290</v>
-      </c>
-      <c r="G25" s="15" t="s">
-        <v>291</v>
       </c>
       <c r="K25" s="15" t="s">
         <v>17</v>
@@ -74909,7 +74909,7 @@
     </row>
     <row r="26" spans="1:29">
       <c r="A26" s="15" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>280</v>
@@ -74918,13 +74918,13 @@
         <v>280</v>
       </c>
       <c r="E26" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="F26" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="G26" s="15" t="s">
         <v>290</v>
-      </c>
-      <c r="G26" s="15" t="s">
-        <v>291</v>
       </c>
       <c r="K26" s="15" t="s">
         <v>17</v>
@@ -74983,7 +74983,7 @@
     </row>
     <row r="27" spans="1:29">
       <c r="A27" s="15" t="s">
-        <v>288</v>
+        <v>298</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>280</v>
@@ -74992,13 +74992,13 @@
         <v>280</v>
       </c>
       <c r="E27" s="15" t="s">
+        <v>288</v>
+      </c>
+      <c r="F27" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="G27" s="15" t="s">
         <v>290</v>
-      </c>
-      <c r="G27" s="15" t="s">
-        <v>291</v>
       </c>
       <c r="K27" s="15" t="s">
         <v>17</v>
@@ -75054,7 +75054,7 @@
     </row>
     <row r="28" spans="1:29">
       <c r="A28" s="15" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>280</v>
@@ -75063,13 +75063,13 @@
         <v>280</v>
       </c>
       <c r="E28" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="F28" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="G28" s="15" t="s">
         <v>293</v>
-      </c>
-      <c r="F28" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="G28" s="15" t="s">
-        <v>295</v>
       </c>
       <c r="K28" s="15" t="s">
         <v>17</v>
@@ -75125,7 +75125,7 @@
     </row>
     <row r="29" spans="1:29">
       <c r="A29" s="15" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>280</v>
@@ -75134,13 +75134,13 @@
         <v>280</v>
       </c>
       <c r="E29" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="F29" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="G29" s="15" t="s">
         <v>293</v>
-      </c>
-      <c r="F29" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="G29" s="15" t="s">
-        <v>295</v>
       </c>
       <c r="K29" s="15" t="s">
         <v>17</v>
@@ -75199,7 +75199,7 @@
     </row>
     <row r="30" spans="1:29">
       <c r="A30" s="15" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>280</v>
@@ -75208,13 +75208,13 @@
         <v>280</v>
       </c>
       <c r="E30" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="F30" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="G30" s="15" t="s">
         <v>293</v>
-      </c>
-      <c r="F30" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="G30" s="15" t="s">
-        <v>295</v>
       </c>
       <c r="K30" s="15" t="s">
         <v>17</v>
@@ -75273,7 +75273,7 @@
     </row>
     <row r="31" spans="1:29">
       <c r="A31" s="15" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>280</v>
@@ -75282,13 +75282,13 @@
         <v>280</v>
       </c>
       <c r="E31" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="F31" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="G31" s="15" t="s">
         <v>293</v>
-      </c>
-      <c r="F31" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="G31" s="15" t="s">
-        <v>295</v>
       </c>
       <c r="K31" s="15" t="s">
         <v>17</v>
@@ -75347,7 +75347,7 @@
     </row>
     <row r="32" spans="1:29">
       <c r="A32" s="15" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>280</v>
@@ -75356,13 +75356,13 @@
         <v>280</v>
       </c>
       <c r="E32" s="15" t="s">
+        <v>291</v>
+      </c>
+      <c r="F32" s="15" t="s">
+        <v>292</v>
+      </c>
+      <c r="G32" s="15" t="s">
         <v>293</v>
-      </c>
-      <c r="F32" s="15" t="s">
-        <v>294</v>
-      </c>
-      <c r="G32" s="15" t="s">
-        <v>295</v>
       </c>
       <c r="K32" s="15" t="s">
         <v>17</v>
@@ -75421,7 +75421,7 @@
     </row>
     <row r="33" spans="1:29">
       <c r="A33" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>280</v>
@@ -75430,13 +75430,13 @@
         <v>280</v>
       </c>
       <c r="E33" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="F33" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="G33" s="15" t="s">
         <v>297</v>
-      </c>
-      <c r="F33" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="G33" s="15" t="s">
-        <v>299</v>
       </c>
       <c r="K33" s="15" t="s">
         <v>17</v>
@@ -75492,7 +75492,7 @@
     </row>
     <row r="34" spans="1:29">
       <c r="A34" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>280</v>
@@ -75501,13 +75501,13 @@
         <v>280</v>
       </c>
       <c r="E34" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="F34" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="G34" s="15" t="s">
         <v>297</v>
-      </c>
-      <c r="F34" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="G34" s="15" t="s">
-        <v>299</v>
       </c>
       <c r="K34" s="15" t="s">
         <v>17</v>
@@ -75566,7 +75566,7 @@
     </row>
     <row r="35" spans="1:29">
       <c r="A35" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>280</v>
@@ -75575,13 +75575,13 @@
         <v>280</v>
       </c>
       <c r="E35" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="F35" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="G35" s="15" t="s">
         <v>297</v>
-      </c>
-      <c r="F35" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="G35" s="15" t="s">
-        <v>299</v>
       </c>
       <c r="K35" s="15" t="s">
         <v>17</v>
@@ -75640,7 +75640,7 @@
     </row>
     <row r="36" spans="1:29">
       <c r="A36" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>280</v>
@@ -75649,13 +75649,13 @@
         <v>280</v>
       </c>
       <c r="E36" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="F36" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="G36" s="15" t="s">
         <v>297</v>
-      </c>
-      <c r="F36" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="G36" s="15" t="s">
-        <v>299</v>
       </c>
       <c r="K36" s="15" t="s">
         <v>17</v>
@@ -75714,7 +75714,7 @@
     </row>
     <row r="37" spans="1:29">
       <c r="A37" s="15" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>280</v>
@@ -75723,13 +75723,13 @@
         <v>280</v>
       </c>
       <c r="E37" s="15" t="s">
+        <v>295</v>
+      </c>
+      <c r="F37" s="15" t="s">
+        <v>296</v>
+      </c>
+      <c r="G37" s="15" t="s">
         <v>297</v>
-      </c>
-      <c r="F37" s="15" t="s">
-        <v>298</v>
-      </c>
-      <c r="G37" s="15" t="s">
-        <v>299</v>
       </c>
       <c r="K37" s="15" t="s">
         <v>17</v>

</xml_diff>